<commit_message>
update shap and tc-python
</commit_message>
<xml_diff>
--- a/04_Model_Saved/NN_full_v3_BO_test_9/MultiTaskModel_NiCrCoVFe_KW99_wt_pct_ML.xlsx
+++ b/04_Model_Saved/NN_full_v3_BO_test_9/MultiTaskModel_NiCrCoVFe_KW99_wt_pct_ML.xlsx
@@ -505,16 +505,16 @@
         <v>10.27148578895017</v>
       </c>
       <c r="G2" t="n">
-        <v>140.5332489013672</v>
+        <v>142.8804626464844</v>
       </c>
       <c r="H2" t="n">
-        <v>31.6042366027832</v>
+        <v>32.14314270019531</v>
       </c>
       <c r="I2" t="n">
-        <v>502.8800048828125</v>
+        <v>505.0473022460938</v>
       </c>
       <c r="J2" t="n">
-        <v>86.56943511962891</v>
+        <v>84.26080322265625</v>
       </c>
     </row>
     <row r="3">
@@ -537,16 +537,16 @@
         <v>10.49540628405087</v>
       </c>
       <c r="G3" t="n">
-        <v>146.2063598632812</v>
+        <v>147.5453338623047</v>
       </c>
       <c r="H3" t="n">
-        <v>31.3714656829834</v>
+        <v>32.31061172485352</v>
       </c>
       <c r="I3" t="n">
-        <v>521.7821655273438</v>
+        <v>519.9776000976562</v>
       </c>
       <c r="J3" t="n">
-        <v>91.53156280517578</v>
+        <v>102.3788757324219</v>
       </c>
     </row>
     <row r="4">
@@ -569,16 +569,16 @@
         <v>11.11292799977388</v>
       </c>
       <c r="G4" t="n">
-        <v>151.6212921142578</v>
+        <v>150.9543914794922</v>
       </c>
       <c r="H4" t="n">
-        <v>31.57857704162598</v>
+        <v>33.08547592163086</v>
       </c>
       <c r="I4" t="n">
-        <v>541.8428955078125</v>
+        <v>544.2020874023438</v>
       </c>
       <c r="J4" t="n">
-        <v>112.5113296508789</v>
+        <v>107.5343170166016</v>
       </c>
     </row>
     <row r="5">
@@ -601,16 +601,16 @@
         <v>11.33579528302992</v>
       </c>
       <c r="G5" t="n">
-        <v>155.5661468505859</v>
+        <v>156.8717193603516</v>
       </c>
       <c r="H5" t="n">
-        <v>36.48318862915039</v>
+        <v>38.1383056640625</v>
       </c>
       <c r="I5" t="n">
-        <v>553.3155517578125</v>
+        <v>553.709716796875</v>
       </c>
       <c r="J5" t="n">
-        <v>123.7189025878906</v>
+        <v>119.4354705810547</v>
       </c>
     </row>
     <row r="6">
@@ -633,16 +633,16 @@
         <v>11.53221857575777</v>
       </c>
       <c r="G6" t="n">
-        <v>162.4016571044922</v>
+        <v>161.7545776367188</v>
       </c>
       <c r="H6" t="n">
-        <v>42.85956573486328</v>
+        <v>41.96193313598633</v>
       </c>
       <c r="I6" t="n">
-        <v>528.9210815429688</v>
+        <v>535.7727661132812</v>
       </c>
       <c r="J6" t="n">
-        <v>152.3361511230469</v>
+        <v>150.2334289550781</v>
       </c>
     </row>
     <row r="7">
@@ -665,16 +665,16 @@
         <v>11.73836346032553</v>
       </c>
       <c r="G7" t="n">
-        <v>127.9208602905273</v>
+        <v>128.0693054199219</v>
       </c>
       <c r="H7" t="n">
-        <v>35.40781784057617</v>
+        <v>33.70592498779297</v>
       </c>
       <c r="I7" t="n">
-        <v>416.7857666015625</v>
+        <v>429.8053283691406</v>
       </c>
       <c r="J7" t="n">
-        <v>93.30745697021484</v>
+        <v>87.16747283935547</v>
       </c>
     </row>
     <row r="8">
@@ -697,16 +697,16 @@
         <v>12.47588443056982</v>
       </c>
       <c r="G8" t="n">
-        <v>133.2911529541016</v>
+        <v>135.1362762451172</v>
       </c>
       <c r="H8" t="n">
-        <v>32.23892211914062</v>
+        <v>34.33587265014648</v>
       </c>
       <c r="I8" t="n">
-        <v>465.5369262695312</v>
+        <v>467.0935363769531</v>
       </c>
       <c r="J8" t="n">
-        <v>88.49763488769531</v>
+        <v>90.19690704345703</v>
       </c>
     </row>
     <row r="9">
@@ -729,16 +729,16 @@
         <v>13.31360035996819</v>
       </c>
       <c r="G9" t="n">
-        <v>141.01416015625</v>
+        <v>140.7048187255859</v>
       </c>
       <c r="H9" t="n">
-        <v>31.5971622467041</v>
+        <v>32.55530166625977</v>
       </c>
       <c r="I9" t="n">
-        <v>490.1704711914062</v>
+        <v>490.3887634277344</v>
       </c>
       <c r="J9" t="n">
-        <v>84.47855377197266</v>
+        <v>83.94367218017578</v>
       </c>
     </row>
     <row r="10">
@@ -761,16 +761,16 @@
         <v>14.04586286313179</v>
       </c>
       <c r="G10" t="n">
-        <v>145.1638336181641</v>
+        <v>144.6791229248047</v>
       </c>
       <c r="H10" t="n">
-        <v>27.86515998840332</v>
+        <v>26.5163745880127</v>
       </c>
       <c r="I10" t="n">
-        <v>507.4932250976562</v>
+        <v>510.056396484375</v>
       </c>
       <c r="J10" t="n">
-        <v>78.78611755371094</v>
+        <v>78.10751342773438</v>
       </c>
     </row>
     <row r="11">
@@ -793,16 +793,16 @@
         <v>14.78596965177877</v>
       </c>
       <c r="G11" t="n">
-        <v>150.4430847167969</v>
+        <v>149.5959777832031</v>
       </c>
       <c r="H11" t="n">
-        <v>26.61432647705078</v>
+        <v>27.48994064331055</v>
       </c>
       <c r="I11" t="n">
-        <v>516.5221557617188</v>
+        <v>520.3779296875</v>
       </c>
       <c r="J11" t="n">
-        <v>92.33889770507812</v>
+        <v>90.37418365478516</v>
       </c>
     </row>
     <row r="12">
@@ -825,16 +825,16 @@
         <v>14.60750023008277</v>
       </c>
       <c r="G12" t="n">
-        <v>154.8320617675781</v>
+        <v>155.1700897216797</v>
       </c>
       <c r="H12" t="n">
-        <v>29.4629955291748</v>
+        <v>29.0160961151123</v>
       </c>
       <c r="I12" t="n">
-        <v>506.739013671875</v>
+        <v>502.6429138183594</v>
       </c>
       <c r="J12" t="n">
-        <v>95.49766540527344</v>
+        <v>102.3632125854492</v>
       </c>
     </row>
     <row r="13">
@@ -857,16 +857,16 @@
         <v>13.93632017907879</v>
       </c>
       <c r="G13" t="n">
-        <v>170.3138427734375</v>
+        <v>170.6553344726562</v>
       </c>
       <c r="H13" t="n">
-        <v>33.39278030395508</v>
+        <v>32.18177795410156</v>
       </c>
       <c r="I13" t="n">
-        <v>481.9498291015625</v>
+        <v>483.3847961425781</v>
       </c>
       <c r="J13" t="n">
-        <v>137.9275665283203</v>
+        <v>128.67626953125</v>
       </c>
     </row>
     <row r="14">
@@ -889,16 +889,16 @@
         <v>13.2060787967079</v>
       </c>
       <c r="G14" t="n">
-        <v>117.0631408691406</v>
+        <v>116.7173156738281</v>
       </c>
       <c r="H14" t="n">
-        <v>31.92207717895508</v>
+        <v>31.8255558013916</v>
       </c>
       <c r="I14" t="n">
-        <v>255.4125823974609</v>
+        <v>254.7527618408203</v>
       </c>
       <c r="J14" t="n">
-        <v>83.63051605224609</v>
+        <v>83.21837615966797</v>
       </c>
     </row>
     <row r="15">
@@ -921,16 +921,16 @@
         <v>14.43724685121477</v>
       </c>
       <c r="G15" t="n">
-        <v>124.2992935180664</v>
+        <v>123.8658828735352</v>
       </c>
       <c r="H15" t="n">
-        <v>37.03987884521484</v>
+        <v>36.62961578369141</v>
       </c>
       <c r="I15" t="n">
-        <v>294.7309265136719</v>
+        <v>295.86328125</v>
       </c>
       <c r="J15" t="n">
-        <v>85.53610229492188</v>
+        <v>86.25227355957031</v>
       </c>
     </row>
     <row r="16">
@@ -953,16 +953,16 @@
         <v>15.77509757365795</v>
       </c>
       <c r="G16" t="n">
-        <v>128.8102264404297</v>
+        <v>128.9159088134766</v>
       </c>
       <c r="H16" t="n">
-        <v>36.25160598754883</v>
+        <v>34.73052215576172</v>
       </c>
       <c r="I16" t="n">
-        <v>351.9001159667969</v>
+        <v>348.5033569335938</v>
       </c>
       <c r="J16" t="n">
-        <v>94.40224456787109</v>
+        <v>95.79824829101562</v>
       </c>
     </row>
     <row r="17">
@@ -985,16 +985,16 @@
         <v>17.01643502058164</v>
       </c>
       <c r="G17" t="n">
-        <v>137.5036315917969</v>
+        <v>138.2591552734375</v>
       </c>
       <c r="H17" t="n">
-        <v>36.01143264770508</v>
+        <v>35.63236236572266</v>
       </c>
       <c r="I17" t="n">
-        <v>422.8345031738281</v>
+        <v>424.6423950195312</v>
       </c>
       <c r="J17" t="n">
-        <v>102.8279876708984</v>
+        <v>102.8576812744141</v>
       </c>
     </row>
     <row r="18">
@@ -1017,16 +1017,16 @@
         <v>17.57324774662381</v>
       </c>
       <c r="G18" t="n">
-        <v>140.3657684326172</v>
+        <v>140.3032073974609</v>
       </c>
       <c r="H18" t="n">
-        <v>29.99698257446289</v>
+        <v>29.81174087524414</v>
       </c>
       <c r="I18" t="n">
-        <v>453.4910888671875</v>
+        <v>454.2892761230469</v>
       </c>
       <c r="J18" t="n">
-        <v>97.32173156738281</v>
+        <v>99.47294616699219</v>
       </c>
     </row>
     <row r="19">
@@ -1049,16 +1049,16 @@
         <v>18.2282289394109</v>
       </c>
       <c r="G19" t="n">
-        <v>144.8411254882812</v>
+        <v>144.9179229736328</v>
       </c>
       <c r="H19" t="n">
-        <v>22.99314308166504</v>
+        <v>24.13729667663574</v>
       </c>
       <c r="I19" t="n">
-        <v>495.2444763183594</v>
+        <v>491.6285400390625</v>
       </c>
       <c r="J19" t="n">
-        <v>86.32498931884766</v>
+        <v>88.19241333007812</v>
       </c>
     </row>
     <row r="20">
@@ -1081,16 +1081,16 @@
         <v>18.05168677518481</v>
       </c>
       <c r="G20" t="n">
-        <v>151.3220672607422</v>
+        <v>152.2935180664062</v>
       </c>
       <c r="H20" t="n">
-        <v>25.38350677490234</v>
+        <v>24.90175819396973</v>
       </c>
       <c r="I20" t="n">
-        <v>495.8152465820312</v>
+        <v>497.2941589355469</v>
       </c>
       <c r="J20" t="n">
-        <v>100.6157302856445</v>
+        <v>93.54551696777344</v>
       </c>
     </row>
     <row r="21">
@@ -1113,16 +1113,16 @@
         <v>17.30316829702608</v>
       </c>
       <c r="G21" t="n">
-        <v>169.7555694580078</v>
+        <v>169.7773132324219</v>
       </c>
       <c r="H21" t="n">
-        <v>28.5236873626709</v>
+        <v>26.39823341369629</v>
       </c>
       <c r="I21" t="n">
-        <v>483.1077575683594</v>
+        <v>478.9127502441406</v>
       </c>
       <c r="J21" t="n">
-        <v>121.1484222412109</v>
+        <v>130.5850524902344</v>
       </c>
     </row>
     <row r="22">
@@ -1145,16 +1145,16 @@
         <v>15.87142913305469</v>
       </c>
       <c r="G22" t="n">
-        <v>233.5515594482422</v>
+        <v>234.3558044433594</v>
       </c>
       <c r="H22" t="n">
-        <v>43.57487869262695</v>
+        <v>41.10518646240234</v>
       </c>
       <c r="I22" t="n">
-        <v>449.1123046875</v>
+        <v>446.4248352050781</v>
       </c>
       <c r="J22" t="n">
-        <v>177.4573516845703</v>
+        <v>170.0016784667969</v>
       </c>
     </row>
     <row r="23">
@@ -1177,16 +1177,16 @@
         <v>16.2842163689804</v>
       </c>
       <c r="G23" t="n">
-        <v>115.8605575561523</v>
+        <v>116.4716033935547</v>
       </c>
       <c r="H23" t="n">
-        <v>35.21152496337891</v>
+        <v>35.94319915771484</v>
       </c>
       <c r="I23" t="n">
-        <v>207.4049987792969</v>
+        <v>206.6993255615234</v>
       </c>
       <c r="J23" t="n">
-        <v>95.30816650390625</v>
+        <v>91.93099212646484</v>
       </c>
     </row>
     <row r="24">
@@ -1209,16 +1209,16 @@
         <v>17.99859633271077</v>
       </c>
       <c r="G24" t="n">
-        <v>121.4489974975586</v>
+        <v>121.291145324707</v>
       </c>
       <c r="H24" t="n">
-        <v>36.28131103515625</v>
+        <v>35.83256149291992</v>
       </c>
       <c r="I24" t="n">
-        <v>256.1204833984375</v>
+        <v>252.6391143798828</v>
       </c>
       <c r="J24" t="n">
-        <v>91.39031982421875</v>
+        <v>94.19733428955078</v>
       </c>
     </row>
     <row r="25">
@@ -1241,16 +1241,16 @@
         <v>19.53665474474453</v>
       </c>
       <c r="G25" t="n">
-        <v>125.7404327392578</v>
+        <v>127.6668243408203</v>
       </c>
       <c r="H25" t="n">
-        <v>33.36998748779297</v>
+        <v>36.89981079101562</v>
       </c>
       <c r="I25" t="n">
-        <v>289.6951599121094</v>
+        <v>290.1314697265625</v>
       </c>
       <c r="J25" t="n">
-        <v>90.9896240234375</v>
+        <v>89.4581298828125</v>
       </c>
     </row>
     <row r="26">
@@ -1273,16 +1273,16 @@
         <v>21.18080958029204</v>
       </c>
       <c r="G26" t="n">
-        <v>133.7445068359375</v>
+        <v>133.9181823730469</v>
       </c>
       <c r="H26" t="n">
-        <v>35.95676422119141</v>
+        <v>36.31747817993164</v>
       </c>
       <c r="I26" t="n">
-        <v>338.0440673828125</v>
+        <v>334.0249633789062</v>
       </c>
       <c r="J26" t="n">
-        <v>90.58865356445312</v>
+        <v>99.53156280517578</v>
       </c>
     </row>
     <row r="27">
@@ -1305,16 +1305,16 @@
         <v>22.36133238808863</v>
       </c>
       <c r="G27" t="n">
-        <v>138.9653930664062</v>
+        <v>140.0730285644531</v>
       </c>
       <c r="H27" t="n">
-        <v>29.95430946350098</v>
+        <v>30.42644691467285</v>
       </c>
       <c r="I27" t="n">
-        <v>393.1442260742188</v>
+        <v>397.5252990722656</v>
       </c>
       <c r="J27" t="n">
-        <v>114.1809616088867</v>
+        <v>109.7086181640625</v>
       </c>
     </row>
     <row r="28">
@@ -1337,16 +1337,16 @@
         <v>22.25528267810615</v>
       </c>
       <c r="G28" t="n">
-        <v>142.4730529785156</v>
+        <v>142.3007354736328</v>
       </c>
       <c r="H28" t="n">
-        <v>22.32204818725586</v>
+        <v>22.0538387298584</v>
       </c>
       <c r="I28" t="n">
-        <v>445.2800598144531</v>
+        <v>445.6835021972656</v>
       </c>
       <c r="J28" t="n">
-        <v>109.400032043457</v>
+        <v>107.9384384155273</v>
       </c>
     </row>
     <row r="29">
@@ -1369,16 +1369,16 @@
         <v>22.11853696692908</v>
       </c>
       <c r="G29" t="n">
-        <v>152.7609710693359</v>
+        <v>152.0797729492188</v>
       </c>
       <c r="H29" t="n">
-        <v>22.96137428283691</v>
+        <v>22.72967720031738</v>
       </c>
       <c r="I29" t="n">
-        <v>477.9927062988281</v>
+        <v>475.8534851074219</v>
       </c>
       <c r="J29" t="n">
-        <v>102.3666381835938</v>
+        <v>108.8017196655273</v>
       </c>
     </row>
     <row r="30">
@@ -1401,16 +1401,16 @@
         <v>21.13587239531939</v>
       </c>
       <c r="G30" t="n">
-        <v>181.8912048339844</v>
+        <v>181.1639251708984</v>
       </c>
       <c r="H30" t="n">
-        <v>27.98550033569336</v>
+        <v>28.08621788024902</v>
       </c>
       <c r="I30" t="n">
-        <v>479.6531677246094</v>
+        <v>470.8873901367188</v>
       </c>
       <c r="J30" t="n">
-        <v>122.2161636352539</v>
+        <v>138.1964111328125</v>
       </c>
     </row>
     <row r="31">
@@ -1433,16 +1433,16 @@
         <v>19.80061812897557</v>
       </c>
       <c r="G31" t="n">
-        <v>246.9253387451172</v>
+        <v>246.7310485839844</v>
       </c>
       <c r="H31" t="n">
-        <v>41.04867935180664</v>
+        <v>42.73271179199219</v>
       </c>
       <c r="I31" t="n">
-        <v>444.370361328125</v>
+        <v>444.4541625976562</v>
       </c>
       <c r="J31" t="n">
-        <v>179.7878875732422</v>
+        <v>185.6873474121094</v>
       </c>
     </row>
     <row r="32">
@@ -1465,16 +1465,16 @@
         <v>20.55168297688286</v>
       </c>
       <c r="G32" t="n">
-        <v>114.1943511962891</v>
+        <v>114.985466003418</v>
       </c>
       <c r="H32" t="n">
-        <v>29.66370391845703</v>
+        <v>31.7579517364502</v>
       </c>
       <c r="I32" t="n">
-        <v>159.4123382568359</v>
+        <v>153.0612030029297</v>
       </c>
       <c r="J32" t="n">
-        <v>100.4605102539062</v>
+        <v>100.3491821289062</v>
       </c>
     </row>
     <row r="33">
@@ -1497,16 +1497,16 @@
         <v>22.96934284445093</v>
       </c>
       <c r="G33" t="n">
-        <v>120.9783096313477</v>
+        <v>121.3505859375</v>
       </c>
       <c r="H33" t="n">
-        <v>35.98047256469727</v>
+        <v>36.63999176025391</v>
       </c>
       <c r="I33" t="n">
-        <v>213.4684295654297</v>
+        <v>211.6167755126953</v>
       </c>
       <c r="J33" t="n">
-        <v>104.9187545776367</v>
+        <v>101.7864990234375</v>
       </c>
     </row>
     <row r="34">
@@ -1529,16 +1529,16 @@
         <v>24.40915250803127</v>
       </c>
       <c r="G34" t="n">
-        <v>125.7099380493164</v>
+        <v>126.8276596069336</v>
       </c>
       <c r="H34" t="n">
-        <v>36.31646728515625</v>
+        <v>36.69324493408203</v>
       </c>
       <c r="I34" t="n">
-        <v>262.8878479003906</v>
+        <v>265.167236328125</v>
       </c>
       <c r="J34" t="n">
-        <v>101.2973861694336</v>
+        <v>99.86502075195312</v>
       </c>
     </row>
     <row r="35">
@@ -1561,16 +1561,16 @@
         <v>26.0811880993595</v>
       </c>
       <c r="G35" t="n">
-        <v>132.7925720214844</v>
+        <v>133.0792846679688</v>
       </c>
       <c r="H35" t="n">
-        <v>36.8427848815918</v>
+        <v>36.49098968505859</v>
       </c>
       <c r="I35" t="n">
-        <v>308.0265197753906</v>
+        <v>306.5359497070312</v>
       </c>
       <c r="J35" t="n">
-        <v>105.0192794799805</v>
+        <v>108.3628692626953</v>
       </c>
     </row>
     <row r="36">
@@ -1593,16 +1593,16 @@
         <v>26.87614780904968</v>
       </c>
       <c r="G36" t="n">
-        <v>139.0648040771484</v>
+        <v>140.2834777832031</v>
       </c>
       <c r="H36" t="n">
-        <v>32.62709045410156</v>
+        <v>32.56547546386719</v>
       </c>
       <c r="I36" t="n">
-        <v>354.9306945800781</v>
+        <v>354.8982849121094</v>
       </c>
       <c r="J36" t="n">
-        <v>114.2610549926758</v>
+        <v>113.9577102661133</v>
       </c>
     </row>
     <row r="37">
@@ -1625,16 +1625,16 @@
         <v>27.16629873490772</v>
       </c>
       <c r="G37" t="n">
-        <v>142.6414642333984</v>
+        <v>144.0287780761719</v>
       </c>
       <c r="H37" t="n">
-        <v>23.56729125976562</v>
+        <v>25.19291496276855</v>
       </c>
       <c r="I37" t="n">
-        <v>396.0415344238281</v>
+        <v>400.09228515625</v>
       </c>
       <c r="J37" t="n">
-        <v>136.0837097167969</v>
+        <v>129.1274719238281</v>
       </c>
     </row>
     <row r="38">
@@ -1657,16 +1657,16 @@
         <v>27.25598473560972</v>
       </c>
       <c r="G38" t="n">
-        <v>154.3629455566406</v>
+        <v>154.6244964599609</v>
       </c>
       <c r="H38" t="n">
-        <v>23.73662757873535</v>
+        <v>22.57598304748535</v>
       </c>
       <c r="I38" t="n">
-        <v>436.6659240722656</v>
+        <v>439.4377136230469</v>
       </c>
       <c r="J38" t="n">
-        <v>134.9339141845703</v>
+        <v>129.8589935302734</v>
       </c>
     </row>
     <row r="39">
@@ -1689,16 +1689,16 @@
         <v>26.04628332899345</v>
       </c>
       <c r="G39" t="n">
-        <v>187.7192077636719</v>
+        <v>186.9638671875</v>
       </c>
       <c r="H39" t="n">
-        <v>31.6436824798584</v>
+        <v>30.44893074035645</v>
       </c>
       <c r="I39" t="n">
-        <v>439.6993713378906</v>
+        <v>439.9128723144531</v>
       </c>
       <c r="J39" t="n">
-        <v>171.2151489257812</v>
+        <v>176.8063354492188</v>
       </c>
     </row>
     <row r="40">
@@ -1721,16 +1721,16 @@
         <v>23.96978635149335</v>
       </c>
       <c r="G40" t="n">
-        <v>258.4585876464844</v>
+        <v>256.0289916992188</v>
       </c>
       <c r="H40" t="n">
-        <v>43.30208206176758</v>
+        <v>40.51065826416016</v>
       </c>
       <c r="I40" t="n">
-        <v>432.5579223632812</v>
+        <v>433.5440673828125</v>
       </c>
       <c r="J40" t="n">
-        <v>197.2715148925781</v>
+        <v>203.0678100585938</v>
       </c>
     </row>
     <row r="41">
@@ -1753,16 +1753,16 @@
         <v>25.6116837653232</v>
       </c>
       <c r="G41" t="n">
-        <v>117.1572036743164</v>
+        <v>114.661994934082</v>
       </c>
       <c r="H41" t="n">
-        <v>34.91884613037109</v>
+        <v>29.29879760742188</v>
       </c>
       <c r="I41" t="n">
-        <v>101.3113708496094</v>
+        <v>104.7073745727539</v>
       </c>
       <c r="J41" t="n">
-        <v>105.3201904296875</v>
+        <v>107.8823776245117</v>
       </c>
     </row>
     <row r="42">
@@ -1785,16 +1785,16 @@
         <v>28.41067839248494</v>
       </c>
       <c r="G42" t="n">
-        <v>121.2093200683594</v>
+        <v>119.9710006713867</v>
       </c>
       <c r="H42" t="n">
-        <v>35.28254699707031</v>
+        <v>32.90065383911133</v>
       </c>
       <c r="I42" t="n">
-        <v>148.6441802978516</v>
+        <v>146.2124786376953</v>
       </c>
       <c r="J42" t="n">
-        <v>115.8625869750977</v>
+        <v>112.5235290527344</v>
       </c>
     </row>
     <row r="43">
@@ -1817,16 +1817,16 @@
         <v>30.68040031937237</v>
       </c>
       <c r="G43" t="n">
-        <v>128.1030120849609</v>
+        <v>126.0315856933594</v>
       </c>
       <c r="H43" t="n">
-        <v>38.15895080566406</v>
+        <v>36.15554428100586</v>
       </c>
       <c r="I43" t="n">
-        <v>214.6107940673828</v>
+        <v>214.6288757324219</v>
       </c>
       <c r="J43" t="n">
-        <v>118.5742645263672</v>
+        <v>118.7913436889648</v>
       </c>
     </row>
     <row r="44">
@@ -1849,16 +1849,16 @@
         <v>32.34762367758118</v>
       </c>
       <c r="G44" t="n">
-        <v>133.7012023925781</v>
+        <v>134.6031799316406</v>
       </c>
       <c r="H44" t="n">
-        <v>37.6923828125</v>
+        <v>37.04384994506836</v>
       </c>
       <c r="I44" t="n">
-        <v>279.7858276367188</v>
+        <v>277.1092224121094</v>
       </c>
       <c r="J44" t="n">
-        <v>119.077522277832</v>
+        <v>120.1916885375977</v>
       </c>
     </row>
     <row r="45">
@@ -1881,16 +1881,16 @@
         <v>33.26712421235609</v>
       </c>
       <c r="G45" t="n">
-        <v>141.1017303466797</v>
+        <v>142.17578125</v>
       </c>
       <c r="H45" t="n">
-        <v>33.32004165649414</v>
+        <v>34.82829666137695</v>
       </c>
       <c r="I45" t="n">
-        <v>324.1600646972656</v>
+        <v>326.1495971679688</v>
       </c>
       <c r="J45" t="n">
-        <v>123.8079376220703</v>
+        <v>123.6895065307617</v>
       </c>
     </row>
     <row r="46">
@@ -1913,16 +1913,16 @@
         <v>33.39925272231932</v>
       </c>
       <c r="G46" t="n">
-        <v>148.6099548339844</v>
+        <v>150.2042541503906</v>
       </c>
       <c r="H46" t="n">
-        <v>26.70205879211426</v>
+        <v>29.46469879150391</v>
       </c>
       <c r="I46" t="n">
-        <v>371.6121215820312</v>
+        <v>373.58740234375</v>
       </c>
       <c r="J46" t="n">
-        <v>146.4331512451172</v>
+        <v>146.1094512939453</v>
       </c>
     </row>
     <row r="47">
@@ -1945,16 +1945,16 @@
         <v>32.83385481517335</v>
       </c>
       <c r="G47" t="n">
-        <v>158.6004028320312</v>
+        <v>157.4096832275391</v>
       </c>
       <c r="H47" t="n">
-        <v>27.68056488037109</v>
+        <v>26.90229225158691</v>
       </c>
       <c r="I47" t="n">
-        <v>403.3045349121094</v>
+        <v>398.7059631347656</v>
       </c>
       <c r="J47" t="n">
-        <v>163.4591217041016</v>
+        <v>165.2471466064453</v>
       </c>
     </row>
     <row r="48">
@@ -1977,16 +1977,16 @@
         <v>31.22587875804939</v>
       </c>
       <c r="G48" t="n">
-        <v>196.7827606201172</v>
+        <v>199.2266998291016</v>
       </c>
       <c r="H48" t="n">
-        <v>33.97626495361328</v>
+        <v>36.078369140625</v>
       </c>
       <c r="I48" t="n">
-        <v>417.8979797363281</v>
+        <v>422.9988403320312</v>
       </c>
       <c r="J48" t="n">
-        <v>191.2711334228516</v>
+        <v>183.7768402099609</v>
       </c>
     </row>
     <row r="49">
@@ -2009,16 +2009,16 @@
         <v>28.00050845971687</v>
       </c>
       <c r="G49" t="n">
-        <v>265.0576171875</v>
+        <v>264.6051940917969</v>
       </c>
       <c r="H49" t="n">
-        <v>44.30284881591797</v>
+        <v>45.21309661865234</v>
       </c>
       <c r="I49" t="n">
-        <v>420.4049072265625</v>
+        <v>422.933837890625</v>
       </c>
       <c r="J49" t="n">
-        <v>218.4091033935547</v>
+        <v>206.9194793701172</v>
       </c>
     </row>
     <row r="50">
@@ -2041,16 +2041,16 @@
         <v>32.75859992753161</v>
       </c>
       <c r="G50" t="n">
-        <v>119.0328674316406</v>
+        <v>118.913330078125</v>
       </c>
       <c r="H50" t="n">
-        <v>32.85251998901367</v>
+        <v>35.18188858032227</v>
       </c>
       <c r="I50" t="n">
-        <v>57.92562484741211</v>
+        <v>53.16790008544922</v>
       </c>
       <c r="J50" t="n">
-        <v>106.7273406982422</v>
+        <v>111.1792678833008</v>
       </c>
     </row>
     <row r="51">
@@ -2073,16 +2073,16 @@
         <v>35.60454595063857</v>
       </c>
       <c r="G51" t="n">
-        <v>125.0112915039062</v>
+        <v>124.9077835083008</v>
       </c>
       <c r="H51" t="n">
-        <v>37.04553604125977</v>
+        <v>36.35508728027344</v>
       </c>
       <c r="I51" t="n">
-        <v>92.2818603515625</v>
+        <v>87.15781402587891</v>
       </c>
       <c r="J51" t="n">
-        <v>122.5761337280273</v>
+        <v>124.0592422485352</v>
       </c>
     </row>
     <row r="52">
@@ -2105,16 +2105,16 @@
         <v>38.13811789539464</v>
       </c>
       <c r="G52" t="n">
-        <v>129.7406616210938</v>
+        <v>129.5819396972656</v>
       </c>
       <c r="H52" t="n">
-        <v>38.56708526611328</v>
+        <v>37.7817497253418</v>
       </c>
       <c r="I52" t="n">
-        <v>132.5335235595703</v>
+        <v>133.0933074951172</v>
       </c>
       <c r="J52" t="n">
-        <v>132.4614105224609</v>
+        <v>136.7314300537109</v>
       </c>
     </row>
     <row r="53">
@@ -2137,16 +2137,16 @@
         <v>39.1380055059179</v>
       </c>
       <c r="G53" t="n">
-        <v>137.2830200195312</v>
+        <v>137.3786468505859</v>
       </c>
       <c r="H53" t="n">
-        <v>37.38027572631836</v>
+        <v>38.45075225830078</v>
       </c>
       <c r="I53" t="n">
-        <v>214.1496734619141</v>
+        <v>214.6918029785156</v>
       </c>
       <c r="J53" t="n">
-        <v>137.7845611572266</v>
+        <v>141.3419494628906</v>
       </c>
     </row>
     <row r="54">
@@ -2169,16 +2169,16 @@
         <v>40.17007780104868</v>
       </c>
       <c r="G54" t="n">
-        <v>145.3065948486328</v>
+        <v>145.5761413574219</v>
       </c>
       <c r="H54" t="n">
-        <v>36.65341949462891</v>
+        <v>35.2869987487793</v>
       </c>
       <c r="I54" t="n">
-        <v>291.2326965332031</v>
+        <v>296.0212097167969</v>
       </c>
       <c r="J54" t="n">
-        <v>144.0903625488281</v>
+        <v>139.8495483398438</v>
       </c>
     </row>
     <row r="55">
@@ -2201,16 +2201,16 @@
         <v>40.31777520333784</v>
       </c>
       <c r="G55" t="n">
-        <v>156.4150695800781</v>
+        <v>152.8242797851562</v>
       </c>
       <c r="H55" t="n">
-        <v>35.89742660522461</v>
+        <v>34.37796020507812</v>
       </c>
       <c r="I55" t="n">
-        <v>344.1335144042969</v>
+        <v>342.0743408203125</v>
       </c>
       <c r="J55" t="n">
-        <v>148.6371765136719</v>
+        <v>148.5781707763672</v>
       </c>
     </row>
     <row r="56">
@@ -2233,16 +2233,16 @@
         <v>38.89328689858721</v>
       </c>
       <c r="G56" t="n">
-        <v>168.73828125</v>
+        <v>168.6741333007812</v>
       </c>
       <c r="H56" t="n">
-        <v>37.21220397949219</v>
+        <v>35.64198684692383</v>
       </c>
       <c r="I56" t="n">
-        <v>380.3355407714844</v>
+        <v>385.9133911132812</v>
       </c>
       <c r="J56" t="n">
-        <v>172.1407165527344</v>
+        <v>170.4989776611328</v>
       </c>
     </row>
     <row r="57">
@@ -2265,16 +2265,16 @@
         <v>36.03490394546852</v>
       </c>
       <c r="G57" t="n">
-        <v>199.9050903320312</v>
+        <v>199.1276245117188</v>
       </c>
       <c r="H57" t="n">
-        <v>37.9974479675293</v>
+        <v>37.11589050292969</v>
       </c>
       <c r="I57" t="n">
-        <v>402.7809753417969</v>
+        <v>402.0811462402344</v>
       </c>
       <c r="J57" t="n">
-        <v>197.5469512939453</v>
+        <v>198.6816558837891</v>
       </c>
     </row>
     <row r="58">
@@ -2297,16 +2297,16 @@
         <v>33.0417017672229</v>
       </c>
       <c r="G58" t="n">
-        <v>265.4825134277344</v>
+        <v>266.2444763183594</v>
       </c>
       <c r="H58" t="n">
-        <v>48.9182014465332</v>
+        <v>48.58882141113281</v>
       </c>
       <c r="I58" t="n">
-        <v>410.9821472167969</v>
+        <v>409.7958984375</v>
       </c>
       <c r="J58" t="n">
-        <v>217.8299255371094</v>
+        <v>220.9768371582031</v>
       </c>
     </row>
     <row r="59">
@@ -2329,16 +2329,16 @@
         <v>43.98768298598323</v>
       </c>
       <c r="G59" t="n">
-        <v>131.9349365234375</v>
+        <v>131.2852630615234</v>
       </c>
       <c r="H59" t="n">
-        <v>42.30546188354492</v>
+        <v>41.43349838256836</v>
       </c>
       <c r="I59" t="n">
-        <v>24.24511528015137</v>
+        <v>21.03071212768555</v>
       </c>
       <c r="J59" t="n">
-        <v>122.2469482421875</v>
+        <v>117.896125793457</v>
       </c>
     </row>
     <row r="60">
@@ -2361,16 +2361,16 @@
         <v>45.7006317110727</v>
       </c>
       <c r="G60" t="n">
-        <v>136.8954467773438</v>
+        <v>137.4062347412109</v>
       </c>
       <c r="H60" t="n">
-        <v>40.12746429443359</v>
+        <v>42.05660247802734</v>
       </c>
       <c r="I60" t="n">
-        <v>54.68921279907227</v>
+        <v>55.63461685180664</v>
       </c>
       <c r="J60" t="n">
-        <v>136.8984069824219</v>
+        <v>132.5423889160156</v>
       </c>
     </row>
     <row r="61">
@@ -2393,16 +2393,16 @@
         <v>46.67965674781412</v>
       </c>
       <c r="G61" t="n">
-        <v>144.3333892822266</v>
+        <v>143.4328308105469</v>
       </c>
       <c r="H61" t="n">
-        <v>43.17168426513672</v>
+        <v>43.91158676147461</v>
       </c>
       <c r="I61" t="n">
-        <v>124.2264099121094</v>
+        <v>126.0830764770508</v>
       </c>
       <c r="J61" t="n">
-        <v>153.1787567138672</v>
+        <v>153.3572235107422</v>
       </c>
     </row>
     <row r="62">
@@ -2425,16 +2425,16 @@
         <v>47.53914448671719</v>
       </c>
       <c r="G62" t="n">
-        <v>147.7690887451172</v>
+        <v>149.4916229248047</v>
       </c>
       <c r="H62" t="n">
-        <v>41.14724731445312</v>
+        <v>45.73701477050781</v>
       </c>
       <c r="I62" t="n">
-        <v>216.2823638916016</v>
+        <v>211.7987670898438</v>
       </c>
       <c r="J62" t="n">
-        <v>166.1926422119141</v>
+        <v>165.9947814941406</v>
       </c>
     </row>
     <row r="63">
@@ -2457,16 +2457,16 @@
         <v>47.07121651777462</v>
       </c>
       <c r="G63" t="n">
-        <v>159.2462005615234</v>
+        <v>157.6045379638672</v>
       </c>
       <c r="H63" t="n">
-        <v>42.72495269775391</v>
+        <v>39.87849426269531</v>
       </c>
       <c r="I63" t="n">
-        <v>300.7759399414062</v>
+        <v>303.538330078125</v>
       </c>
       <c r="J63" t="n">
-        <v>170.0784454345703</v>
+        <v>166.0636291503906</v>
       </c>
     </row>
     <row r="64">
@@ -2489,16 +2489,16 @@
         <v>45.67156598130153</v>
       </c>
       <c r="G64" t="n">
-        <v>175.452880859375</v>
+        <v>176.8026428222656</v>
       </c>
       <c r="H64" t="n">
-        <v>44.26882553100586</v>
+        <v>49.50154113769531</v>
       </c>
       <c r="I64" t="n">
-        <v>361.3939514160156</v>
+        <v>359.3987121582031</v>
       </c>
       <c r="J64" t="n">
-        <v>170.9430541992188</v>
+        <v>170.7235717773438</v>
       </c>
     </row>
     <row r="65">
@@ -2521,16 +2521,16 @@
         <v>42.51104340916319</v>
       </c>
       <c r="G65" t="n">
-        <v>207.5819091796875</v>
+        <v>203.2075958251953</v>
       </c>
       <c r="H65" t="n">
-        <v>48.47676849365234</v>
+        <v>45.13428497314453</v>
       </c>
       <c r="I65" t="n">
-        <v>375.6427612304688</v>
+        <v>384.80615234375</v>
       </c>
       <c r="J65" t="n">
-        <v>200.5066833496094</v>
+        <v>199.9920654296875</v>
       </c>
     </row>
     <row r="66">
@@ -2553,16 +2553,16 @@
         <v>54.37577254606605</v>
       </c>
       <c r="G66" t="n">
-        <v>144.8886871337891</v>
+        <v>144.9655151367188</v>
       </c>
       <c r="H66" t="n">
-        <v>47.43221282958984</v>
+        <v>51.40160751342773</v>
       </c>
       <c r="I66" t="n">
-        <v>-13.92716503143311</v>
+        <v>-14.52151679992676</v>
       </c>
       <c r="J66" t="n">
-        <v>123.7480850219727</v>
+        <v>121.9946517944336</v>
       </c>
     </row>
     <row r="67">
@@ -2585,16 +2585,16 @@
         <v>55.07062752917076</v>
       </c>
       <c r="G67" t="n">
-        <v>152.6881561279297</v>
+        <v>151.2734222412109</v>
       </c>
       <c r="H67" t="n">
-        <v>58.43179321289062</v>
+        <v>54.50032043457031</v>
       </c>
       <c r="I67" t="n">
-        <v>33.32210159301758</v>
+        <v>40.38976287841797</v>
       </c>
       <c r="J67" t="n">
-        <v>147.509033203125</v>
+        <v>151.8598937988281</v>
       </c>
     </row>
     <row r="68">
@@ -2617,16 +2617,16 @@
         <v>54.82432856758766</v>
       </c>
       <c r="G68" t="n">
-        <v>156.7550811767578</v>
+        <v>154.5999450683594</v>
       </c>
       <c r="H68" t="n">
-        <v>52.6277961730957</v>
+        <v>49.96806716918945</v>
       </c>
       <c r="I68" t="n">
-        <v>121.7443618774414</v>
+        <v>118.2431793212891</v>
       </c>
       <c r="J68" t="n">
-        <v>175.4471588134766</v>
+        <v>173.0519714355469</v>
       </c>
     </row>
     <row r="69">
@@ -2649,16 +2649,16 @@
         <v>54.18769809434324</v>
       </c>
       <c r="G69" t="n">
-        <v>168.9586944580078</v>
+        <v>170.5404968261719</v>
       </c>
       <c r="H69" t="n">
-        <v>54.14697265625</v>
+        <v>55.21120834350586</v>
       </c>
       <c r="I69" t="n">
-        <v>228.5310974121094</v>
+        <v>237.9041442871094</v>
       </c>
       <c r="J69" t="n">
-        <v>192.2873382568359</v>
+        <v>191.1373748779297</v>
       </c>
     </row>
     <row r="70">
@@ -2681,16 +2681,16 @@
         <v>51.347187815424</v>
       </c>
       <c r="G70" t="n">
-        <v>183.2640686035156</v>
+        <v>184.9205322265625</v>
       </c>
       <c r="H70" t="n">
-        <v>55.02800369262695</v>
+        <v>56.38514709472656</v>
       </c>
       <c r="I70" t="n">
-        <v>320.3285827636719</v>
+        <v>319.74365234375</v>
       </c>
       <c r="J70" t="n">
-        <v>185.0646362304688</v>
+        <v>183.4980926513672</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update model to take empty inputs
</commit_message>
<xml_diff>
--- a/04_Model_Saved/NN_full_v3_BO_test_9/MultiTaskModel_NiCrCoVFe_KW99_wt_pct_ML.xlsx
+++ b/04_Model_Saved/NN_full_v3_BO_test_9/MultiTaskModel_NiCrCoVFe_KW99_wt_pct_ML.xlsx
@@ -505,16 +505,16 @@
         <v>10.27148578895017</v>
       </c>
       <c r="G2" t="n">
-        <v>142.8804626464844</v>
+        <v>398.1259765625</v>
       </c>
       <c r="H2" t="n">
-        <v>32.14314270019531</v>
+        <v>27.01040649414062</v>
       </c>
       <c r="I2" t="n">
-        <v>505.0473022460938</v>
+        <v>477.260009765625</v>
       </c>
       <c r="J2" t="n">
-        <v>84.26080322265625</v>
+        <v>53.77014541625977</v>
       </c>
     </row>
     <row r="3">
@@ -537,16 +537,16 @@
         <v>10.49540628405087</v>
       </c>
       <c r="G3" t="n">
-        <v>147.5453338623047</v>
+        <v>403.0327758789062</v>
       </c>
       <c r="H3" t="n">
-        <v>32.31061172485352</v>
+        <v>27.9195728302002</v>
       </c>
       <c r="I3" t="n">
-        <v>519.9776000976562</v>
+        <v>477.33447265625</v>
       </c>
       <c r="J3" t="n">
-        <v>102.3788757324219</v>
+        <v>48.6143913269043</v>
       </c>
     </row>
     <row r="4">
@@ -569,16 +569,16 @@
         <v>11.11292799977388</v>
       </c>
       <c r="G4" t="n">
-        <v>150.9543914794922</v>
+        <v>405.1096801757812</v>
       </c>
       <c r="H4" t="n">
-        <v>33.08547592163086</v>
+        <v>25.76400184631348</v>
       </c>
       <c r="I4" t="n">
-        <v>544.2020874023438</v>
+        <v>478.2184753417969</v>
       </c>
       <c r="J4" t="n">
-        <v>107.5343170166016</v>
+        <v>49.50567626953125</v>
       </c>
     </row>
     <row r="5">
@@ -601,16 +601,16 @@
         <v>11.33579528302992</v>
       </c>
       <c r="G5" t="n">
-        <v>156.8717193603516</v>
+        <v>408.9818115234375</v>
       </c>
       <c r="H5" t="n">
-        <v>38.1383056640625</v>
+        <v>24.48388671875</v>
       </c>
       <c r="I5" t="n">
-        <v>553.709716796875</v>
+        <v>473.5812377929688</v>
       </c>
       <c r="J5" t="n">
-        <v>119.4354705810547</v>
+        <v>53.30754089355469</v>
       </c>
     </row>
     <row r="6">
@@ -633,16 +633,16 @@
         <v>11.53221857575777</v>
       </c>
       <c r="G6" t="n">
-        <v>161.7545776367188</v>
+        <v>412.66064453125</v>
       </c>
       <c r="H6" t="n">
-        <v>41.96193313598633</v>
+        <v>23.39294242858887</v>
       </c>
       <c r="I6" t="n">
-        <v>535.7727661132812</v>
+        <v>465.3410949707031</v>
       </c>
       <c r="J6" t="n">
-        <v>150.2334289550781</v>
+        <v>59.19172286987305</v>
       </c>
     </row>
     <row r="7">
@@ -665,16 +665,16 @@
         <v>11.73836346032553</v>
       </c>
       <c r="G7" t="n">
-        <v>128.0693054199219</v>
+        <v>382.5882873535156</v>
       </c>
       <c r="H7" t="n">
-        <v>33.70592498779297</v>
+        <v>28.43268013000488</v>
       </c>
       <c r="I7" t="n">
-        <v>429.8053283691406</v>
+        <v>444.3815612792969</v>
       </c>
       <c r="J7" t="n">
-        <v>87.16747283935547</v>
+        <v>63.25116348266602</v>
       </c>
     </row>
     <row r="8">
@@ -697,16 +697,16 @@
         <v>12.47588443056982</v>
       </c>
       <c r="G8" t="n">
-        <v>135.1362762451172</v>
+        <v>388.7621765136719</v>
       </c>
       <c r="H8" t="n">
-        <v>34.33587265014648</v>
+        <v>28.43271255493164</v>
       </c>
       <c r="I8" t="n">
-        <v>467.0935363769531</v>
+        <v>454.9195251464844</v>
       </c>
       <c r="J8" t="n">
-        <v>90.19690704345703</v>
+        <v>62.44813537597656</v>
       </c>
     </row>
     <row r="9">
@@ -729,16 +729,16 @@
         <v>13.31360035996819</v>
       </c>
       <c r="G9" t="n">
-        <v>140.7048187255859</v>
+        <v>393.1926574707031</v>
       </c>
       <c r="H9" t="n">
-        <v>32.55530166625977</v>
+        <v>25.77258491516113</v>
       </c>
       <c r="I9" t="n">
-        <v>490.3887634277344</v>
+        <v>462.656982421875</v>
       </c>
       <c r="J9" t="n">
-        <v>83.94367218017578</v>
+        <v>54.33234405517578</v>
       </c>
     </row>
     <row r="10">
@@ -761,16 +761,16 @@
         <v>14.04586286313179</v>
       </c>
       <c r="G10" t="n">
-        <v>144.6791229248047</v>
+        <v>398.5402526855469</v>
       </c>
       <c r="H10" t="n">
-        <v>26.5163745880127</v>
+        <v>26.66025161743164</v>
       </c>
       <c r="I10" t="n">
-        <v>510.056396484375</v>
+        <v>465.3640747070312</v>
       </c>
       <c r="J10" t="n">
-        <v>78.10751342773438</v>
+        <v>56.68073654174805</v>
       </c>
     </row>
     <row r="11">
@@ -793,16 +793,16 @@
         <v>14.78596965177877</v>
       </c>
       <c r="G11" t="n">
-        <v>149.5959777832031</v>
+        <v>403.7288818359375</v>
       </c>
       <c r="H11" t="n">
-        <v>27.48994064331055</v>
+        <v>24.84552192687988</v>
       </c>
       <c r="I11" t="n">
-        <v>520.3779296875</v>
+        <v>464.3366088867188</v>
       </c>
       <c r="J11" t="n">
-        <v>90.37418365478516</v>
+        <v>54.12376403808594</v>
       </c>
     </row>
     <row r="12">
@@ -825,16 +825,16 @@
         <v>14.60750023008277</v>
       </c>
       <c r="G12" t="n">
-        <v>155.1700897216797</v>
+        <v>412.3948059082031</v>
       </c>
       <c r="H12" t="n">
-        <v>29.0160961151123</v>
+        <v>24.6420783996582</v>
       </c>
       <c r="I12" t="n">
-        <v>502.6429138183594</v>
+        <v>463.9165649414062</v>
       </c>
       <c r="J12" t="n">
-        <v>102.3632125854492</v>
+        <v>57.08152008056641</v>
       </c>
     </row>
     <row r="13">
@@ -857,16 +857,16 @@
         <v>13.93632017907879</v>
       </c>
       <c r="G13" t="n">
-        <v>170.6553344726562</v>
+        <v>424.3629455566406</v>
       </c>
       <c r="H13" t="n">
-        <v>32.18177795410156</v>
+        <v>24.00087928771973</v>
       </c>
       <c r="I13" t="n">
-        <v>483.3847961425781</v>
+        <v>448.2315063476562</v>
       </c>
       <c r="J13" t="n">
-        <v>128.67626953125</v>
+        <v>69.34293365478516</v>
       </c>
     </row>
     <row r="14">
@@ -889,16 +889,16 @@
         <v>13.2060787967079</v>
       </c>
       <c r="G14" t="n">
-        <v>116.7173156738281</v>
+        <v>368.1524353027344</v>
       </c>
       <c r="H14" t="n">
-        <v>31.8255558013916</v>
+        <v>27.97834587097168</v>
       </c>
       <c r="I14" t="n">
-        <v>254.7527618408203</v>
+        <v>382.9455871582031</v>
       </c>
       <c r="J14" t="n">
-        <v>83.21837615966797</v>
+        <v>86.08547210693359</v>
       </c>
     </row>
     <row r="15">
@@ -921,16 +921,16 @@
         <v>14.43724685121477</v>
       </c>
       <c r="G15" t="n">
-        <v>123.8658828735352</v>
+        <v>375.8694152832031</v>
       </c>
       <c r="H15" t="n">
-        <v>36.62961578369141</v>
+        <v>28.27974700927734</v>
       </c>
       <c r="I15" t="n">
-        <v>295.86328125</v>
+        <v>410.5798950195312</v>
       </c>
       <c r="J15" t="n">
-        <v>86.25227355957031</v>
+        <v>73.89263916015625</v>
       </c>
     </row>
     <row r="16">
@@ -953,16 +953,16 @@
         <v>15.77509757365795</v>
       </c>
       <c r="G16" t="n">
-        <v>128.9159088134766</v>
+        <v>379.32421875</v>
       </c>
       <c r="H16" t="n">
-        <v>34.73052215576172</v>
+        <v>28.25710105895996</v>
       </c>
       <c r="I16" t="n">
-        <v>348.5033569335938</v>
+        <v>429.6340942382812</v>
       </c>
       <c r="J16" t="n">
-        <v>95.79824829101562</v>
+        <v>64.95188903808594</v>
       </c>
     </row>
     <row r="17">
@@ -985,16 +985,16 @@
         <v>17.01643502058164</v>
       </c>
       <c r="G17" t="n">
-        <v>138.2591552734375</v>
+        <v>387.8291931152344</v>
       </c>
       <c r="H17" t="n">
-        <v>35.63236236572266</v>
+        <v>27.64620780944824</v>
       </c>
       <c r="I17" t="n">
-        <v>424.6423950195312</v>
+        <v>443.8576965332031</v>
       </c>
       <c r="J17" t="n">
-        <v>102.8576812744141</v>
+        <v>59.06442642211914</v>
       </c>
     </row>
     <row r="18">
@@ -1017,16 +1017,16 @@
         <v>17.57324774662381</v>
       </c>
       <c r="G18" t="n">
-        <v>140.3032073974609</v>
+        <v>392.5246887207031</v>
       </c>
       <c r="H18" t="n">
-        <v>29.81174087524414</v>
+        <v>26.5245532989502</v>
       </c>
       <c r="I18" t="n">
-        <v>454.2892761230469</v>
+        <v>450.2022399902344</v>
       </c>
       <c r="J18" t="n">
-        <v>99.47294616699219</v>
+        <v>61.19875717163086</v>
       </c>
     </row>
     <row r="19">
@@ -1049,16 +1049,16 @@
         <v>18.2282289394109</v>
       </c>
       <c r="G19" t="n">
-        <v>144.9179229736328</v>
+        <v>401.2491760253906</v>
       </c>
       <c r="H19" t="n">
-        <v>24.13729667663574</v>
+        <v>27.44148445129395</v>
       </c>
       <c r="I19" t="n">
-        <v>491.6285400390625</v>
+        <v>454.8536987304688</v>
       </c>
       <c r="J19" t="n">
-        <v>88.19241333007812</v>
+        <v>56.44916534423828</v>
       </c>
     </row>
     <row r="20">
@@ -1081,16 +1081,16 @@
         <v>18.05168677518481</v>
       </c>
       <c r="G20" t="n">
-        <v>152.2935180664062</v>
+        <v>410.4702758789062</v>
       </c>
       <c r="H20" t="n">
-        <v>24.90175819396973</v>
+        <v>24.41758918762207</v>
       </c>
       <c r="I20" t="n">
-        <v>497.2941589355469</v>
+        <v>455.0971984863281</v>
       </c>
       <c r="J20" t="n">
-        <v>93.54551696777344</v>
+        <v>56.87409591674805</v>
       </c>
     </row>
     <row r="21">
@@ -1113,16 +1113,16 @@
         <v>17.30316829702608</v>
       </c>
       <c r="G21" t="n">
-        <v>169.7773132324219</v>
+        <v>425.2373046875</v>
       </c>
       <c r="H21" t="n">
-        <v>26.39823341369629</v>
+        <v>24.80557441711426</v>
       </c>
       <c r="I21" t="n">
-        <v>478.9127502441406</v>
+        <v>440.2408447265625</v>
       </c>
       <c r="J21" t="n">
-        <v>130.5850524902344</v>
+        <v>70.75784301757812</v>
       </c>
     </row>
     <row r="22">
@@ -1145,16 +1145,16 @@
         <v>15.87142913305469</v>
       </c>
       <c r="G22" t="n">
-        <v>234.3558044433594</v>
+        <v>445.6087036132812</v>
       </c>
       <c r="H22" t="n">
-        <v>41.10518646240234</v>
+        <v>26.41068840026855</v>
       </c>
       <c r="I22" t="n">
-        <v>446.4248352050781</v>
+        <v>421.9258422851562</v>
       </c>
       <c r="J22" t="n">
-        <v>170.0016784667969</v>
+        <v>81.25815582275391</v>
       </c>
     </row>
     <row r="23">
@@ -1177,16 +1177,16 @@
         <v>16.2842163689804</v>
       </c>
       <c r="G23" t="n">
-        <v>116.4716033935547</v>
+        <v>363.1999206542969</v>
       </c>
       <c r="H23" t="n">
-        <v>35.94319915771484</v>
+        <v>28.20826148986816</v>
       </c>
       <c r="I23" t="n">
-        <v>206.6993255615234</v>
+        <v>349.7908630371094</v>
       </c>
       <c r="J23" t="n">
-        <v>91.93099212646484</v>
+        <v>89.15886688232422</v>
       </c>
     </row>
     <row r="24">
@@ -1209,16 +1209,16 @@
         <v>17.99859633271077</v>
       </c>
       <c r="G24" t="n">
-        <v>121.291145324707</v>
+        <v>368.5528869628906</v>
       </c>
       <c r="H24" t="n">
-        <v>35.83256149291992</v>
+        <v>27.62983512878418</v>
       </c>
       <c r="I24" t="n">
-        <v>252.6391143798828</v>
+        <v>381.3911743164062</v>
       </c>
       <c r="J24" t="n">
-        <v>94.19733428955078</v>
+        <v>81.29314422607422</v>
       </c>
     </row>
     <row r="25">
@@ -1241,16 +1241,16 @@
         <v>19.53665474474453</v>
       </c>
       <c r="G25" t="n">
-        <v>127.6668243408203</v>
+        <v>375.1595764160156</v>
       </c>
       <c r="H25" t="n">
-        <v>36.89981079101562</v>
+        <v>27.59327507019043</v>
       </c>
       <c r="I25" t="n">
-        <v>290.1314697265625</v>
+        <v>401.1213989257812</v>
       </c>
       <c r="J25" t="n">
-        <v>89.4581298828125</v>
+        <v>74.40888977050781</v>
       </c>
     </row>
     <row r="26">
@@ -1273,16 +1273,16 @@
         <v>21.18080958029204</v>
       </c>
       <c r="G26" t="n">
-        <v>133.9181823730469</v>
+        <v>382.3030090332031</v>
       </c>
       <c r="H26" t="n">
-        <v>36.31747817993164</v>
+        <v>28.20405387878418</v>
       </c>
       <c r="I26" t="n">
-        <v>334.0249633789062</v>
+        <v>416.0938415527344</v>
       </c>
       <c r="J26" t="n">
-        <v>99.53156280517578</v>
+        <v>72.64133453369141</v>
       </c>
     </row>
     <row r="27">
@@ -1305,16 +1305,16 @@
         <v>22.36133238808863</v>
       </c>
       <c r="G27" t="n">
-        <v>140.0730285644531</v>
+        <v>389.591796875</v>
       </c>
       <c r="H27" t="n">
-        <v>30.42644691467285</v>
+        <v>26.14640998840332</v>
       </c>
       <c r="I27" t="n">
-        <v>397.5252990722656</v>
+        <v>433.1531066894531</v>
       </c>
       <c r="J27" t="n">
-        <v>109.7086181640625</v>
+        <v>67.19808197021484</v>
       </c>
     </row>
     <row r="28">
@@ -1337,16 +1337,16 @@
         <v>22.25528267810615</v>
       </c>
       <c r="G28" t="n">
-        <v>142.3007354736328</v>
+        <v>397.2207946777344</v>
       </c>
       <c r="H28" t="n">
-        <v>22.0538387298584</v>
+        <v>26.28407287597656</v>
       </c>
       <c r="I28" t="n">
-        <v>445.6835021972656</v>
+        <v>440.4262390136719</v>
       </c>
       <c r="J28" t="n">
-        <v>107.9384384155273</v>
+        <v>61.23685455322266</v>
       </c>
     </row>
     <row r="29">
@@ -1369,16 +1369,16 @@
         <v>22.11853696692908</v>
       </c>
       <c r="G29" t="n">
-        <v>152.0797729492188</v>
+        <v>412.2499084472656</v>
       </c>
       <c r="H29" t="n">
-        <v>22.72967720031738</v>
+        <v>25.43990707397461</v>
       </c>
       <c r="I29" t="n">
-        <v>475.8534851074219</v>
+        <v>443.7078247070312</v>
       </c>
       <c r="J29" t="n">
-        <v>108.8017196655273</v>
+        <v>58.79115676879883</v>
       </c>
     </row>
     <row r="30">
@@ -1401,16 +1401,16 @@
         <v>21.13587239531939</v>
       </c>
       <c r="G30" t="n">
-        <v>181.1639251708984</v>
+        <v>429.0813293457031</v>
       </c>
       <c r="H30" t="n">
-        <v>28.08621788024902</v>
+        <v>25.46852874755859</v>
       </c>
       <c r="I30" t="n">
-        <v>470.8873901367188</v>
+        <v>438.8312072753906</v>
       </c>
       <c r="J30" t="n">
-        <v>138.1964111328125</v>
+        <v>67.19949340820312</v>
       </c>
     </row>
     <row r="31">
@@ -1433,16 +1433,16 @@
         <v>19.80061812897557</v>
       </c>
       <c r="G31" t="n">
-        <v>246.7310485839844</v>
+        <v>447.7859497070312</v>
       </c>
       <c r="H31" t="n">
-        <v>42.73271179199219</v>
+        <v>23.9729175567627</v>
       </c>
       <c r="I31" t="n">
-        <v>444.4541625976562</v>
+        <v>417.5845336914062</v>
       </c>
       <c r="J31" t="n">
-        <v>185.6873474121094</v>
+        <v>87.48397827148438</v>
       </c>
     </row>
     <row r="32">
@@ -1465,16 +1465,16 @@
         <v>20.55168297688286</v>
       </c>
       <c r="G32" t="n">
-        <v>114.985466003418</v>
+        <v>359.213134765625</v>
       </c>
       <c r="H32" t="n">
-        <v>31.7579517364502</v>
+        <v>28.32734489440918</v>
       </c>
       <c r="I32" t="n">
-        <v>153.0612030029297</v>
+        <v>317.5141296386719</v>
       </c>
       <c r="J32" t="n">
-        <v>100.3491821289062</v>
+        <v>98.64371490478516</v>
       </c>
     </row>
     <row r="33">
@@ -1497,16 +1497,16 @@
         <v>22.96934284445093</v>
       </c>
       <c r="G33" t="n">
-        <v>121.3505859375</v>
+        <v>366.6471862792969</v>
       </c>
       <c r="H33" t="n">
-        <v>36.63999176025391</v>
+        <v>27.3071174621582</v>
       </c>
       <c r="I33" t="n">
-        <v>211.6167755126953</v>
+        <v>342.8547668457031</v>
       </c>
       <c r="J33" t="n">
-        <v>101.7864990234375</v>
+        <v>94.98149108886719</v>
       </c>
     </row>
     <row r="34">
@@ -1529,16 +1529,16 @@
         <v>24.40915250803127</v>
       </c>
       <c r="G34" t="n">
-        <v>126.8276596069336</v>
+        <v>370.2333984375</v>
       </c>
       <c r="H34" t="n">
-        <v>36.69324493408203</v>
+        <v>27.46042251586914</v>
       </c>
       <c r="I34" t="n">
-        <v>265.167236328125</v>
+        <v>371.8676147460938</v>
       </c>
       <c r="J34" t="n">
-        <v>99.86502075195312</v>
+        <v>83.18350219726562</v>
       </c>
     </row>
     <row r="35">
@@ -1561,16 +1561,16 @@
         <v>26.0811880993595</v>
       </c>
       <c r="G35" t="n">
-        <v>133.0792846679688</v>
+        <v>379.580810546875</v>
       </c>
       <c r="H35" t="n">
-        <v>36.49098968505859</v>
+        <v>27.94532585144043</v>
       </c>
       <c r="I35" t="n">
-        <v>306.5359497070312</v>
+        <v>394.2941284179688</v>
       </c>
       <c r="J35" t="n">
-        <v>108.3628692626953</v>
+        <v>74.88552856445312</v>
       </c>
     </row>
     <row r="36">
@@ -1593,16 +1593,16 @@
         <v>26.87614780904968</v>
       </c>
       <c r="G36" t="n">
-        <v>140.2834777832031</v>
+        <v>386.1780395507812</v>
       </c>
       <c r="H36" t="n">
-        <v>32.56547546386719</v>
+        <v>27.84191131591797</v>
       </c>
       <c r="I36" t="n">
-        <v>354.8982849121094</v>
+        <v>416.1960144042969</v>
       </c>
       <c r="J36" t="n">
-        <v>113.9577102661133</v>
+        <v>71.09192657470703</v>
       </c>
     </row>
     <row r="37">
@@ -1625,16 +1625,16 @@
         <v>27.16629873490772</v>
       </c>
       <c r="G37" t="n">
-        <v>144.0287780761719</v>
+        <v>393.2438354492188</v>
       </c>
       <c r="H37" t="n">
-        <v>25.19291496276855</v>
+        <v>25.46757888793945</v>
       </c>
       <c r="I37" t="n">
-        <v>400.09228515625</v>
+        <v>419.0548400878906</v>
       </c>
       <c r="J37" t="n">
-        <v>129.1274719238281</v>
+        <v>69.82829284667969</v>
       </c>
     </row>
     <row r="38">
@@ -1657,16 +1657,16 @@
         <v>27.25598473560972</v>
       </c>
       <c r="G38" t="n">
-        <v>154.6244964599609</v>
+        <v>406.7008972167969</v>
       </c>
       <c r="H38" t="n">
-        <v>22.57598304748535</v>
+        <v>24.46286582946777</v>
       </c>
       <c r="I38" t="n">
-        <v>439.4377136230469</v>
+        <v>427.4778442382812</v>
       </c>
       <c r="J38" t="n">
-        <v>129.8589935302734</v>
+        <v>72.47047424316406</v>
       </c>
     </row>
     <row r="39">
@@ -1689,16 +1689,16 @@
         <v>26.04628332899345</v>
       </c>
       <c r="G39" t="n">
-        <v>186.9638671875</v>
+        <v>428.0379638671875</v>
       </c>
       <c r="H39" t="n">
-        <v>30.44893074035645</v>
+        <v>26.8080883026123</v>
       </c>
       <c r="I39" t="n">
-        <v>439.9128723144531</v>
+        <v>421.4319152832031</v>
       </c>
       <c r="J39" t="n">
-        <v>176.8063354492188</v>
+        <v>76.64485931396484</v>
       </c>
     </row>
     <row r="40">
@@ -1721,16 +1721,16 @@
         <v>23.96978635149335</v>
       </c>
       <c r="G40" t="n">
-        <v>256.0289916992188</v>
+        <v>450.9182434082031</v>
       </c>
       <c r="H40" t="n">
-        <v>40.51065826416016</v>
+        <v>25.53032875061035</v>
       </c>
       <c r="I40" t="n">
-        <v>433.5440673828125</v>
+        <v>400.5530700683594</v>
       </c>
       <c r="J40" t="n">
-        <v>203.0678100585938</v>
+        <v>92.24122619628906</v>
       </c>
     </row>
     <row r="41">
@@ -1753,16 +1753,16 @@
         <v>25.6116837653232</v>
       </c>
       <c r="G41" t="n">
-        <v>114.661994934082</v>
+        <v>360.4913330078125</v>
       </c>
       <c r="H41" t="n">
-        <v>29.29879760742188</v>
+        <v>28.02543449401855</v>
       </c>
       <c r="I41" t="n">
-        <v>104.7073745727539</v>
+        <v>296.0922241210938</v>
       </c>
       <c r="J41" t="n">
-        <v>107.8823776245117</v>
+        <v>96.97303771972656</v>
       </c>
     </row>
     <row r="42">
@@ -1785,16 +1785,16 @@
         <v>28.41067839248494</v>
       </c>
       <c r="G42" t="n">
-        <v>119.9710006713867</v>
+        <v>363.5075988769531</v>
       </c>
       <c r="H42" t="n">
-        <v>32.90065383911133</v>
+        <v>28.22387504577637</v>
       </c>
       <c r="I42" t="n">
-        <v>146.2124786376953</v>
+        <v>319.1215209960938</v>
       </c>
       <c r="J42" t="n">
-        <v>112.5235290527344</v>
+        <v>91.51718902587891</v>
       </c>
     </row>
     <row r="43">
@@ -1817,16 +1817,16 @@
         <v>30.68040031937237</v>
       </c>
       <c r="G43" t="n">
-        <v>126.0315856933594</v>
+        <v>369.1275634765625</v>
       </c>
       <c r="H43" t="n">
-        <v>36.15554428100586</v>
+        <v>27.08649635314941</v>
       </c>
       <c r="I43" t="n">
-        <v>214.6288757324219</v>
+        <v>334.0909729003906</v>
       </c>
       <c r="J43" t="n">
-        <v>118.7913436889648</v>
+        <v>90.02082061767578</v>
       </c>
     </row>
     <row r="44">
@@ -1849,16 +1849,16 @@
         <v>32.34762367758118</v>
       </c>
       <c r="G44" t="n">
-        <v>134.6031799316406</v>
+        <v>374.1165161132812</v>
       </c>
       <c r="H44" t="n">
-        <v>37.04384994506836</v>
+        <v>27.69235610961914</v>
       </c>
       <c r="I44" t="n">
-        <v>277.1092224121094</v>
+        <v>365.1660766601562</v>
       </c>
       <c r="J44" t="n">
-        <v>120.1916885375977</v>
+        <v>79.88849639892578</v>
       </c>
     </row>
     <row r="45">
@@ -1881,16 +1881,16 @@
         <v>33.26712421235609</v>
       </c>
       <c r="G45" t="n">
-        <v>142.17578125</v>
+        <v>382.7475891113281</v>
       </c>
       <c r="H45" t="n">
-        <v>34.82829666137695</v>
+        <v>27.78489112854004</v>
       </c>
       <c r="I45" t="n">
-        <v>326.1495971679688</v>
+        <v>381.8503723144531</v>
       </c>
       <c r="J45" t="n">
-        <v>123.6895065307617</v>
+        <v>77.33165740966797</v>
       </c>
     </row>
     <row r="46">
@@ -1913,16 +1913,16 @@
         <v>33.39925272231932</v>
       </c>
       <c r="G46" t="n">
-        <v>150.2042541503906</v>
+        <v>394.8126525878906</v>
       </c>
       <c r="H46" t="n">
-        <v>29.46469879150391</v>
+        <v>27.3180980682373</v>
       </c>
       <c r="I46" t="n">
-        <v>373.58740234375</v>
+        <v>403.4883728027344</v>
       </c>
       <c r="J46" t="n">
-        <v>146.1094512939453</v>
+        <v>75.71820831298828</v>
       </c>
     </row>
     <row r="47">
@@ -1945,16 +1945,16 @@
         <v>32.83385481517335</v>
       </c>
       <c r="G47" t="n">
-        <v>157.4096832275391</v>
+        <v>406.127685546875</v>
       </c>
       <c r="H47" t="n">
-        <v>26.90229225158691</v>
+        <v>26.54232215881348</v>
       </c>
       <c r="I47" t="n">
-        <v>398.7059631347656</v>
+        <v>411.6073303222656</v>
       </c>
       <c r="J47" t="n">
-        <v>165.2471466064453</v>
+        <v>71.67802429199219</v>
       </c>
     </row>
     <row r="48">
@@ -1977,16 +1977,16 @@
         <v>31.22587875804939</v>
       </c>
       <c r="G48" t="n">
-        <v>199.2266998291016</v>
+        <v>427.6911315917969</v>
       </c>
       <c r="H48" t="n">
-        <v>36.078369140625</v>
+        <v>25.55732727050781</v>
       </c>
       <c r="I48" t="n">
-        <v>422.9988403320312</v>
+        <v>408.298828125</v>
       </c>
       <c r="J48" t="n">
-        <v>183.7768402099609</v>
+        <v>81.12566375732422</v>
       </c>
     </row>
     <row r="49">
@@ -2009,16 +2009,16 @@
         <v>28.00050845971687</v>
       </c>
       <c r="G49" t="n">
-        <v>264.6051940917969</v>
+        <v>451.606201171875</v>
       </c>
       <c r="H49" t="n">
-        <v>45.21309661865234</v>
+        <v>25.93669700622559</v>
       </c>
       <c r="I49" t="n">
-        <v>422.933837890625</v>
+        <v>400.8568115234375</v>
       </c>
       <c r="J49" t="n">
-        <v>206.9194793701172</v>
+        <v>89.54064178466797</v>
       </c>
     </row>
     <row r="50">
@@ -2041,16 +2041,16 @@
         <v>32.75859992753161</v>
       </c>
       <c r="G50" t="n">
-        <v>118.913330078125</v>
+        <v>359.1517333984375</v>
       </c>
       <c r="H50" t="n">
-        <v>35.18188858032227</v>
+        <v>27.78376388549805</v>
       </c>
       <c r="I50" t="n">
-        <v>53.16790008544922</v>
+        <v>272.7567138671875</v>
       </c>
       <c r="J50" t="n">
-        <v>111.1792678833008</v>
+        <v>98.04290771484375</v>
       </c>
     </row>
     <row r="51">
@@ -2073,16 +2073,16 @@
         <v>35.60454595063857</v>
       </c>
       <c r="G51" t="n">
-        <v>124.9077835083008</v>
+        <v>364.1138916015625</v>
       </c>
       <c r="H51" t="n">
-        <v>36.35508728027344</v>
+        <v>27.7718391418457</v>
       </c>
       <c r="I51" t="n">
-        <v>87.15781402587891</v>
+        <v>293.1388549804688</v>
       </c>
       <c r="J51" t="n">
-        <v>124.0592422485352</v>
+        <v>100.2650756835938</v>
       </c>
     </row>
     <row r="52">
@@ -2105,16 +2105,16 @@
         <v>38.13811789539464</v>
       </c>
       <c r="G52" t="n">
-        <v>129.5819396972656</v>
+        <v>367.4444885253906</v>
       </c>
       <c r="H52" t="n">
-        <v>37.7817497253418</v>
+        <v>27.62353897094727</v>
       </c>
       <c r="I52" t="n">
-        <v>133.0933074951172</v>
+        <v>305.184814453125</v>
       </c>
       <c r="J52" t="n">
-        <v>136.7314300537109</v>
+        <v>97.78956604003906</v>
       </c>
     </row>
     <row r="53">
@@ -2137,16 +2137,16 @@
         <v>39.1380055059179</v>
       </c>
       <c r="G53" t="n">
-        <v>137.3786468505859</v>
+        <v>374.1478576660156</v>
       </c>
       <c r="H53" t="n">
-        <v>38.45075225830078</v>
+        <v>27.19668197631836</v>
       </c>
       <c r="I53" t="n">
-        <v>214.6918029785156</v>
+        <v>325.7828369140625</v>
       </c>
       <c r="J53" t="n">
-        <v>141.3419494628906</v>
+        <v>93.8709716796875</v>
       </c>
     </row>
     <row r="54">
@@ -2169,16 +2169,16 @@
         <v>40.17007780104868</v>
       </c>
       <c r="G54" t="n">
-        <v>145.5761413574219</v>
+        <v>381.4328002929688</v>
       </c>
       <c r="H54" t="n">
-        <v>35.2869987487793</v>
+        <v>26.78518676757812</v>
       </c>
       <c r="I54" t="n">
-        <v>296.0212097167969</v>
+        <v>348.3912963867188</v>
       </c>
       <c r="J54" t="n">
-        <v>139.8495483398438</v>
+        <v>82.96847534179688</v>
       </c>
     </row>
     <row r="55">
@@ -2201,16 +2201,16 @@
         <v>40.31777520333784</v>
       </c>
       <c r="G55" t="n">
-        <v>152.8242797851562</v>
+        <v>389.7665100097656</v>
       </c>
       <c r="H55" t="n">
-        <v>34.37796020507812</v>
+        <v>27.37735939025879</v>
       </c>
       <c r="I55" t="n">
-        <v>342.0743408203125</v>
+        <v>370.6318054199219</v>
       </c>
       <c r="J55" t="n">
-        <v>148.5781707763672</v>
+        <v>76.5948486328125</v>
       </c>
     </row>
     <row r="56">
@@ -2233,16 +2233,16 @@
         <v>38.89328689858721</v>
       </c>
       <c r="G56" t="n">
-        <v>168.6741333007812</v>
+        <v>404.561279296875</v>
       </c>
       <c r="H56" t="n">
-        <v>35.64198684692383</v>
+        <v>27.50343132019043</v>
       </c>
       <c r="I56" t="n">
-        <v>385.9133911132812</v>
+        <v>389.0888061523438</v>
       </c>
       <c r="J56" t="n">
-        <v>170.4989776611328</v>
+        <v>79.48863983154297</v>
       </c>
     </row>
     <row r="57">
@@ -2265,16 +2265,16 @@
         <v>36.03490394546852</v>
       </c>
       <c r="G57" t="n">
-        <v>199.1276245117188</v>
+        <v>424.84228515625</v>
       </c>
       <c r="H57" t="n">
-        <v>37.11589050292969</v>
+        <v>26.05106735229492</v>
       </c>
       <c r="I57" t="n">
-        <v>402.0811462402344</v>
+        <v>394.3933715820312</v>
       </c>
       <c r="J57" t="n">
-        <v>198.6816558837891</v>
+        <v>81.06951141357422</v>
       </c>
     </row>
     <row r="58">
@@ -2297,16 +2297,16 @@
         <v>33.0417017672229</v>
       </c>
       <c r="G58" t="n">
-        <v>266.2444763183594</v>
+        <v>450.9777221679688</v>
       </c>
       <c r="H58" t="n">
-        <v>48.58882141113281</v>
+        <v>25.50094032287598</v>
       </c>
       <c r="I58" t="n">
-        <v>409.7958984375</v>
+        <v>385.2449645996094</v>
       </c>
       <c r="J58" t="n">
-        <v>220.9768371582031</v>
+        <v>97.62964630126953</v>
       </c>
     </row>
     <row r="59">
@@ -2329,16 +2329,16 @@
         <v>43.98768298598323</v>
       </c>
       <c r="G59" t="n">
-        <v>131.2852630615234</v>
+        <v>363.4585266113281</v>
       </c>
       <c r="H59" t="n">
-        <v>41.43349838256836</v>
+        <v>27.91312599182129</v>
       </c>
       <c r="I59" t="n">
-        <v>21.03071212768555</v>
+        <v>262.7206420898438</v>
       </c>
       <c r="J59" t="n">
-        <v>117.896125793457</v>
+        <v>99.8597412109375</v>
       </c>
     </row>
     <row r="60">
@@ -2361,16 +2361,16 @@
         <v>45.7006317110727</v>
       </c>
       <c r="G60" t="n">
-        <v>137.4062347412109</v>
+        <v>366.885986328125</v>
       </c>
       <c r="H60" t="n">
-        <v>42.05660247802734</v>
+        <v>28.75186920166016</v>
       </c>
       <c r="I60" t="n">
-        <v>55.63461685180664</v>
+        <v>277.6995544433594</v>
       </c>
       <c r="J60" t="n">
-        <v>132.5423889160156</v>
+        <v>97.35076904296875</v>
       </c>
     </row>
     <row r="61">
@@ -2393,16 +2393,16 @@
         <v>46.67965674781412</v>
       </c>
       <c r="G61" t="n">
-        <v>143.4328308105469</v>
+        <v>373.3158569335938</v>
       </c>
       <c r="H61" t="n">
-        <v>43.91158676147461</v>
+        <v>27.58979988098145</v>
       </c>
       <c r="I61" t="n">
-        <v>126.0830764770508</v>
+        <v>297.0329284667969</v>
       </c>
       <c r="J61" t="n">
-        <v>153.3572235107422</v>
+        <v>94.16371917724609</v>
       </c>
     </row>
     <row r="62">
@@ -2425,16 +2425,16 @@
         <v>47.53914448671719</v>
       </c>
       <c r="G62" t="n">
-        <v>149.4916229248047</v>
+        <v>379.7358703613281</v>
       </c>
       <c r="H62" t="n">
-        <v>45.73701477050781</v>
+        <v>26.34573936462402</v>
       </c>
       <c r="I62" t="n">
-        <v>211.7987670898438</v>
+        <v>309.5865173339844</v>
       </c>
       <c r="J62" t="n">
-        <v>165.9947814941406</v>
+        <v>89.04312133789062</v>
       </c>
     </row>
     <row r="63">
@@ -2457,16 +2457,16 @@
         <v>47.07121651777462</v>
       </c>
       <c r="G63" t="n">
-        <v>157.6045379638672</v>
+        <v>389.122314453125</v>
       </c>
       <c r="H63" t="n">
-        <v>39.87849426269531</v>
+        <v>28.51152229309082</v>
       </c>
       <c r="I63" t="n">
-        <v>303.538330078125</v>
+        <v>336.3158569335938</v>
       </c>
       <c r="J63" t="n">
-        <v>166.0636291503906</v>
+        <v>84.84140777587891</v>
       </c>
     </row>
     <row r="64">
@@ -2489,16 +2489,16 @@
         <v>45.67156598130153</v>
       </c>
       <c r="G64" t="n">
-        <v>176.8026428222656</v>
+        <v>400.1449890136719</v>
       </c>
       <c r="H64" t="n">
-        <v>49.50154113769531</v>
+        <v>28.3798770904541</v>
       </c>
       <c r="I64" t="n">
-        <v>359.3987121582031</v>
+        <v>368.1322326660156</v>
       </c>
       <c r="J64" t="n">
-        <v>170.7235717773438</v>
+        <v>84.30812835693359</v>
       </c>
     </row>
     <row r="65">
@@ -2521,16 +2521,16 @@
         <v>42.51104340916319</v>
       </c>
       <c r="G65" t="n">
-        <v>203.2075958251953</v>
+        <v>419.9383239746094</v>
       </c>
       <c r="H65" t="n">
-        <v>45.13428497314453</v>
+        <v>25.64868927001953</v>
       </c>
       <c r="I65" t="n">
-        <v>384.80615234375</v>
+        <v>379.0342407226562</v>
       </c>
       <c r="J65" t="n">
-        <v>199.9920654296875</v>
+        <v>81.54350280761719</v>
       </c>
     </row>
     <row r="66">
@@ -2553,16 +2553,16 @@
         <v>54.37577254606605</v>
       </c>
       <c r="G66" t="n">
-        <v>144.9655151367188</v>
+        <v>368.814208984375</v>
       </c>
       <c r="H66" t="n">
-        <v>51.40160751342773</v>
+        <v>28.72645950317383</v>
       </c>
       <c r="I66" t="n">
-        <v>-14.52151679992676</v>
+        <v>225.6248474121094</v>
       </c>
       <c r="J66" t="n">
-        <v>121.9946517944336</v>
+        <v>104.3029022216797</v>
       </c>
     </row>
     <row r="67">
@@ -2585,16 +2585,16 @@
         <v>55.07062752917076</v>
       </c>
       <c r="G67" t="n">
-        <v>151.2734222412109</v>
+        <v>372.7352600097656</v>
       </c>
       <c r="H67" t="n">
-        <v>54.50032043457031</v>
+        <v>27.70173072814941</v>
       </c>
       <c r="I67" t="n">
-        <v>40.38976287841797</v>
+        <v>248.9956207275391</v>
       </c>
       <c r="J67" t="n">
-        <v>151.8598937988281</v>
+        <v>104.537956237793</v>
       </c>
     </row>
     <row r="68">
@@ -2617,16 +2617,16 @@
         <v>54.82432856758766</v>
       </c>
       <c r="G68" t="n">
-        <v>154.5999450683594</v>
+        <v>379.1201171875</v>
       </c>
       <c r="H68" t="n">
-        <v>49.96806716918945</v>
+        <v>27.28972244262695</v>
       </c>
       <c r="I68" t="n">
-        <v>118.2431793212891</v>
+        <v>274.8077392578125</v>
       </c>
       <c r="J68" t="n">
-        <v>173.0519714355469</v>
+        <v>97.98152160644531</v>
       </c>
     </row>
     <row r="69">
@@ -2649,16 +2649,16 @@
         <v>54.18769809434324</v>
       </c>
       <c r="G69" t="n">
-        <v>170.5404968261719</v>
+        <v>386.3962707519531</v>
       </c>
       <c r="H69" t="n">
-        <v>55.21120834350586</v>
+        <v>28.37163543701172</v>
       </c>
       <c r="I69" t="n">
-        <v>237.9041442871094</v>
+        <v>303.657958984375</v>
       </c>
       <c r="J69" t="n">
-        <v>191.1373748779297</v>
+        <v>95.28525543212891</v>
       </c>
     </row>
     <row r="70">
@@ -2681,16 +2681,16 @@
         <v>51.347187815424</v>
       </c>
       <c r="G70" t="n">
-        <v>184.9205322265625</v>
+        <v>399.3856201171875</v>
       </c>
       <c r="H70" t="n">
-        <v>56.38514709472656</v>
+        <v>26.54878807067871</v>
       </c>
       <c r="I70" t="n">
-        <v>319.74365234375</v>
+        <v>340.0702514648438</v>
       </c>
       <c r="J70" t="n">
-        <v>183.4980926513672</v>
+        <v>86.49823760986328</v>
       </c>
     </row>
   </sheetData>

</xml_diff>